<commit_message>
weight frequency of connections by total connections
</commit_message>
<xml_diff>
--- a/CurrentData/policycombos.xlsx
+++ b/CurrentData/policycombos.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="21">
   <si>
     <t>P1</t>
   </si>
@@ -77,6 +77,12 @@
   <si>
     <t>Vulnerable</t>
   </si>
+  <si>
+    <t>Weighted by degree centrality of P1</t>
+  </si>
+  <si>
+    <t>C22/392</t>
+  </si>
 </sst>
 </file>
 
@@ -122,7 +128,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,15 +434,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,8 +455,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -457,8 +469,11 @@
       <c r="C2">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0.15308151093439365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -468,8 +483,11 @@
       <c r="C3">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0.1172962226640159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -479,8 +497,11 @@
       <c r="C4">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0.10934393638170974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -490,8 +511,11 @@
       <c r="C5">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0.1073558648111332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -501,8 +525,11 @@
       <c r="C6">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0.17263843648208468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -512,8 +539,11 @@
       <c r="C7">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0.12755102040816327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -523,8 +553,11 @@
       <c r="C8">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>8.9463220675944338E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -534,8 +567,11 @@
       <c r="C9">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0.16356877323420074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -545,8 +581,11 @@
       <c r="C10">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0.18103448275862069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -556,8 +595,11 @@
       <c r="C11">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0.12883435582822086</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -567,8 +609,11 @@
       <c r="C12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>7.9522862823061632E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -578,8 +623,11 @@
       <c r="C13">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0.1165644171779141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -589,8 +637,11 @@
       <c r="C14">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0.11400651465798045</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -600,8 +651,11 @@
       <c r="C15">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>6.9582504970178927E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -611,8 +665,11 @@
       <c r="C16">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0.10097719869706841</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -622,8 +679,11 @@
       <c r="C17">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>9.5092024539877307E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -633,8 +693,11 @@
       <c r="C18">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0.13043478260869565</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -644,8 +707,11 @@
       <c r="C19">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0.10344827586206896</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -655,8 +721,11 @@
       <c r="C20">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>8.8957055214723926E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -666,8 +735,11 @@
       <c r="C21">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -677,8 +749,11 @@
       <c r="C22">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -688,8 +763,11 @@
       <c r="C23">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>5.5666003976143144E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -699,8 +777,11 @@
       <c r="C24">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>0.1761006289308176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -710,8 +791,11 @@
       <c r="C25">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>5.3677932405566599E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -721,8 +805,11 @@
       <c r="C26">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0.11304347826086956</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -732,8 +819,11 @@
       <c r="C27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>0.1306532663316583</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -743,8 +833,11 @@
       <c r="C28">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>5.168986083499006E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -754,8 +847,11 @@
       <c r="C29">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>7.9754601226993863E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -765,8 +861,11 @@
       <c r="C30">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>9.2936802973977689E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -776,8 +875,11 @@
       <c r="C31">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>9.2936802973977689E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -787,8 +889,11 @@
       <c r="C32">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>6.1224489795918366E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -798,8 +903,11 @@
       <c r="C33">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>8.9219330855018583E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -809,8 +917,11 @@
       <c r="C34">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>4.7713717693836977E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -820,8 +931,11 @@
       <c r="C35">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>8.1784386617100371E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -831,8 +945,11 @@
       <c r="C36">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>4.37375745526839E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -842,8 +959,11 @@
       <c r="C37">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>6.7484662576687116E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -853,8 +973,11 @@
       <c r="C38">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>5.3571428571428568E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -864,8 +987,11 @@
       <c r="C39">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>8.6206896551724144E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -875,8 +1001,11 @@
       <c r="C40">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>6.1349693251533742E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -886,8 +1015,11 @@
       <c r="C41">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>8.2608695652173908E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -897,8 +1029,11 @@
       <c r="C42">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>8.1896551724137928E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -908,8 +1043,11 @@
       <c r="C43">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>0.12413793103448276</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -919,8 +1057,11 @@
       <c r="C44">
         <v>18</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>5.8631921824104233E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -930,8 +1071,11 @@
       <c r="C45">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -941,8 +1085,11 @@
       <c r="C46">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>7.3913043478260873E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -952,8 +1099,11 @@
       <c r="C47">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>8.5427135678391955E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -963,8 +1113,11 @@
       <c r="C48">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>0.1103448275862069</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -974,8 +1127,11 @@
       <c r="C49">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>0.1103448275862069</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -985,8 +1141,11 @@
       <c r="C50">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>5.6034482758620691E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -996,8 +1155,11 @@
       <c r="C51">
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>4.8327137546468404E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -1007,8 +1169,11 @@
       <c r="C52">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>4.8327137546468404E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -1018,8 +1183,11 @@
       <c r="C53">
         <v>13</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>4.2345276872964167E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -1029,8 +1197,11 @@
       <c r="C54">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>4.2345276872964167E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -1040,8 +1211,11 @@
       <c r="C55">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>4.2345276872964167E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -1051,8 +1225,11 @@
       <c r="C56">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>3.9877300613496931E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1062,8 +1239,11 @@
       <c r="C57">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>5.2173913043478258E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -1073,8 +1253,11 @@
       <c r="C58">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>4.4609665427509292E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -1084,8 +1267,11 @@
       <c r="C59">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>4.4609665427509292E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -1095,8 +1281,11 @@
       <c r="C60">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>8.2758620689655171E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -1106,8 +1295,11 @@
       <c r="C61">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>8.2758620689655171E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -1117,8 +1309,11 @@
       <c r="C62">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>3.9087947882736153E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -1128,8 +1323,11 @@
       <c r="C63">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>2.8061224489795918E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -1139,8 +1337,11 @@
       <c r="C64">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>4.7413793103448273E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -1150,8 +1351,11 @@
       <c r="C65">
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>3.3742331288343558E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -1161,8 +1365,11 @@
       <c r="C66">
         <v>11</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>3.3742331288343558E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -1172,8 +1379,11 @@
       <c r="C67">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>4.3478260869565216E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -1183,8 +1393,11 @@
       <c r="C68">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>2.5510204081632654E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -1194,8 +1407,11 @@
       <c r="C69">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>6.8965517241379309E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -1205,8 +1421,11 @@
       <c r="C70">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>3.2573289902280131E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -1216,8 +1435,11 @@
       <c r="C71">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>3.0674846625766871E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -1227,8 +1449,11 @@
       <c r="C72">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>3.9130434782608699E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -1238,8 +1463,11 @@
       <c r="C73">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -1249,8 +1477,11 @@
       <c r="C74">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>4.5226130653266333E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -1260,8 +1491,11 @@
       <c r="C75">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>4.5226130653266333E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -1271,8 +1505,11 @@
       <c r="C76">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>5.6603773584905662E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -1282,8 +1519,11 @@
       <c r="C77">
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>2.7607361963190184E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -1293,8 +1533,11 @@
       <c r="C78">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>1.7167381974248927E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -1304,8 +1547,11 @@
       <c r="C79">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>4.0201005025125629E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -1315,8 +1561,11 @@
       <c r="C80">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>2.9739776951672861E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -1326,8 +1575,11 @@
       <c r="C81">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>5.5172413793103448E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -1337,8 +1589,11 @@
       <c r="C82">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>2.4539877300613498E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -1348,8 +1603,11 @@
       <c r="C83">
         <v>7</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>3.017241379310345E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -1359,8 +1617,11 @@
       <c r="C84">
         <v>7</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>3.017241379310345E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -1370,8 +1631,11 @@
       <c r="C85">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>3.017241379310345E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -1381,8 +1645,11 @@
       <c r="C86">
         <v>6</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>2.2304832713754646E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -1392,8 +1659,11 @@
       <c r="C87">
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>7.3170731707317069E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>15</v>
       </c>
@@ -1403,8 +1673,11 @@
       <c r="C88">
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>1.9543973941368076E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -1414,8 +1687,11 @@
       <c r="C89">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -1425,8 +1701,11 @@
       <c r="C90">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>3.7735849056603772E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -1436,8 +1715,11 @@
       <c r="C91">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>3.7735849056603772E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -1447,8 +1729,11 @@
       <c r="C92">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>2.1739130434782608E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -1458,8 +1743,11 @@
       <c r="C93">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>1.7241379310344827E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -1469,8 +1757,11 @@
       <c r="C94">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -1480,8 +1771,11 @@
       <c r="C95">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>17</v>
       </c>
@@ -1491,8 +1785,11 @@
       <c r="C96">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>9.9403578528827041E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>17</v>
       </c>
@@ -1502,8 +1799,11 @@
       <c r="C97">
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>9.9403578528827041E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -1513,8 +1813,11 @@
       <c r="C98">
         <v>4</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>4.878048780487805E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -1524,8 +1827,11 @@
       <c r="C99">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>3.6585365853658534E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -1535,8 +1841,11 @@
       <c r="C100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>2.0689655172413793E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -1546,8 +1855,11 @@
       <c r="C101">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>2.0689655172413793E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>10</v>
       </c>
@@ -1557,8 +1869,11 @@
       <c r="C102">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>1.8518518518518517E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -1568,8 +1883,11 @@
       <c r="C103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>1.2578616352201259E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -1579,8 +1897,11 @@
       <c r="C104">
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>1.2578616352201259E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -1590,8 +1911,11 @@
       <c r="C105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>2.5510204081632651E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -1601,8 +1925,11 @@
       <c r="C106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>4.3103448275862068E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -1612,8 +1939,11 @@
       <c r="C107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>5.0251256281407036E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>14</v>
       </c>
@@ -1623,8 +1953,11 @@
       <c r="C108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>3.7174721189591076E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -1634,8 +1967,11 @@
       <c r="C109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>1.2195121951219513E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -1645,8 +1981,11 @@
       <c r="C110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>6.8965517241379309E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>10</v>
       </c>
@@ -1656,8 +1995,11 @@
       <c r="C111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>6.1728395061728392E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>17</v>
       </c>
@@ -1667,8 +2009,11 @@
       <c r="C112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>1.9880715705765406E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>18</v>
       </c>
@@ -1677,6 +2022,9 @@
       </c>
       <c r="C113">
         <v>1</v>
+      </c>
+      <c r="D113">
+        <v>3.0674846625766872E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>